<commit_message>
File aggiornato: rimane da sistemare il problema di
# formattare la colonna con il numero del run
#run_number = df_data['Path'].str.split('.').str[0]
#run_number = run_number.str.split('_').str[-1]
#run_number.name= 'Run_Number'
#run_number = pd.to_numeric(run_number)
</commit_message>
<xml_diff>
--- a/documents/CalcolAr-OT-T9-new_pycalcolar.xlsx
+++ b/documents/CalcolAr-OT-T9-new_pycalcolar.xlsx
@@ -623,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CG11"/>
+  <dimension ref="A1:CG6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -891,253 +891,253 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>105</v>
+        <v>246</v>
       </c>
       <c r="D2">
-        <v>1850</v>
+        <v>143.381</v>
       </c>
       <c r="E2">
-        <v>1.1</v>
+        <v>0.05</v>
       </c>
       <c r="F2">
-        <v>3.332464933560954e-07</v>
+        <v>6.421875815344305e-12</v>
       </c>
       <c r="G2">
-        <v>0.013</v>
+        <v>0.018</v>
       </c>
       <c r="H2">
-        <v>6.343191776504066e-07</v>
+        <v>4.237173313727776e-12</v>
       </c>
       <c r="I2">
-        <v>0.013</v>
+        <v>0.00025</v>
       </c>
       <c r="J2">
-        <v>0.002793626730819474</v>
+        <v>1.841141782264091e-11</v>
       </c>
       <c r="K2">
-        <v>0.000242</v>
+        <v>8.847744999999998e-05</v>
       </c>
       <c r="L2">
-        <v>3.167067493117071e-06</v>
+        <v>1.864374356372312e-11</v>
       </c>
       <c r="M2">
-        <v>0.004070000000000001</v>
+        <v>0.0006817114999999999</v>
       </c>
       <c r="N2">
-        <v>1849.91022</v>
+        <v>143.372563515</v>
       </c>
       <c r="O2">
-        <v>1.100000018181818</v>
+        <v>0.05000039999840002</v>
       </c>
       <c r="P2">
-        <v>0.0005946234613384741</v>
+        <v>0.0003487445489748034</v>
       </c>
       <c r="Q2">
-        <v>2.657</v>
+        <v>0.192045</v>
       </c>
       <c r="R2">
-        <v>0.0130034610777285</v>
+        <v>0.018002499826413</v>
       </c>
       <c r="S2">
-        <v>0.004894038794779262</v>
+        <v>0.09374104937078809</v>
       </c>
       <c r="T2">
-        <v>2.529</v>
+        <v>0.127707</v>
       </c>
       <c r="U2">
-        <v>0.01300038460969521</v>
+        <v>0.0002692582403567252</v>
       </c>
       <c r="V2">
-        <v>0.005140523768167342</v>
+        <v>0.002108406276529283</v>
       </c>
       <c r="W2">
-        <v>0.07188</v>
+        <v>0.004403341624499998</v>
       </c>
       <c r="X2">
-        <v>0.0005917465673749194</v>
+        <v>0.0008048777914432119</v>
       </c>
       <c r="Y2">
-        <v>0.008232423029701161</v>
+        <v>0.1827879506247954</v>
       </c>
       <c r="Z2">
-        <v>6.3138</v>
+        <v>0.5708830207500001</v>
       </c>
       <c r="AA2">
-        <v>0.004070049139752493</v>
+        <v>0.0006835426608722018</v>
       </c>
       <c r="AB2">
-        <v>0.0006446275047914873</v>
+        <v>0.00119734277606329</v>
       </c>
       <c r="AC2">
-        <v>8.031712361485972</v>
+        <v>130.0430761721729</v>
       </c>
       <c r="AD2">
-        <v>19292.70616693757</v>
+        <v>0.9690721073699309</v>
       </c>
       <c r="AE2">
-        <v>9646.853083468786</v>
+        <v>0.9845360536849654</v>
       </c>
       <c r="AF2">
-        <v>4823.926541734393</v>
+        <v>0.9922680268424827</v>
       </c>
       <c r="AG2">
-        <v>121810.2881968104</v>
+        <v>0.5532268119799145</v>
       </c>
       <c r="AH2">
-        <v>134035.3490093758</v>
+        <v>251555.4930038796</v>
       </c>
       <c r="AI2">
-        <v>24396.89144809256</v>
+        <v>0.1257321458079459</v>
       </c>
       <c r="AJ2">
-        <v>67017.67450468813</v>
+        <v>125777.7465019398</v>
       </c>
       <c r="AK2">
-        <v>12817.17282138828</v>
+        <v>0.1905601132149646</v>
       </c>
       <c r="AL2">
-        <v>33508.83725234432</v>
+        <v>62888.87325103975</v>
       </c>
       <c r="AM2">
-        <v>107447181.9545951</v>
+        <v>0.5463328730753981</v>
       </c>
       <c r="AN2">
-        <v>100526.5117570321</v>
+        <v>188666.6197529595</v>
       </c>
       <c r="AO2">
-        <v>71989.61190957876</v>
+        <v>0.0003660430249605168</v>
       </c>
       <c r="AP2">
-        <v>100526.5117570332</v>
+        <v>188666.61975296</v>
       </c>
       <c r="AQ2">
-        <v>7236864568.012526</v>
+        <v>69.06010020344908</v>
       </c>
       <c r="AR2">
-        <v>-59172.43908819048</v>
+        <v>0.1901940701900041</v>
       </c>
       <c r="AS2">
-        <v>7249597864.523247</v>
+        <v>11984.3097892293</v>
       </c>
       <c r="AT2">
-        <v>27399.03139842176</v>
+        <v>0.0001393148826342265</v>
       </c>
       <c r="AU2">
-        <v>100526.5117570332</v>
+        <v>188666.61975296</v>
       </c>
       <c r="AV2">
-        <v>2754329052.004767</v>
+        <v>26.28406798787987</v>
       </c>
       <c r="AW2">
-        <v>94411.25679838867</v>
+        <v>0.5530874970972803</v>
       </c>
       <c r="AX2">
-        <v>16557580913.94932</v>
+        <v>139167.2459126655</v>
       </c>
       <c r="AY2">
-        <v>175377.189918225</v>
+        <v>251618.8607463458</v>
       </c>
       <c r="AZ2">
-        <v>28187424.82972692</v>
+        <v>165.129803133364</v>
       </c>
       <c r="BA2">
-        <v>4943431357668.708</v>
+        <v>41549772.93968541</v>
       </c>
       <c r="BB2">
-        <v>-28185574.91950692</v>
+        <v>-21.75723961836405</v>
       </c>
       <c r="BC2">
-        <v>4943431357668.708</v>
+        <v>41549772.93968541</v>
       </c>
       <c r="BD2">
-        <v>-15236.1853103914</v>
+        <v>-0.1517531603324353</v>
       </c>
       <c r="BE2">
-        <v>15238.1853103914</v>
+        <v>2.151753160332436</v>
       </c>
       <c r="BF2">
-        <v>2672430119.189618</v>
+        <v>541421.6788101966</v>
       </c>
       <c r="BG2">
-        <v>-175388.7004890369</v>
+        <v>-1909698.733317971</v>
       </c>
       <c r="BH2">
-        <v>-45883.43348000706</v>
+        <v>-0.1051484010576677</v>
       </c>
       <c r="BI2">
-        <v>4273034167.014439</v>
+        <v>128485.7927556021</v>
       </c>
       <c r="BJ2">
-        <v>-93128.03866075851</v>
+        <v>-1221947.185722161</v>
       </c>
       <c r="BK2">
-        <v>4.809766572e-08</v>
+        <v>4.831655390455499e-09</v>
       </c>
       <c r="BL2">
-        <v>2.860000047272727e-11</v>
+        <v>1.685013479946081e-12</v>
       </c>
       <c r="BM2">
-        <v>-0.0007328249479071799</v>
+        <v>-7.332189751388686e-10</v>
       </c>
       <c r="BN2">
-        <v>128.5292152993864</v>
+        <v>0.001400227348067398</v>
       </c>
       <c r="BO2">
-        <v>0.01116670251078384</v>
+        <v>4.038645341851056e-07</v>
       </c>
       <c r="BP2">
-        <v>0.9493347510827848</v>
+        <v>3.583692644962788</v>
       </c>
       <c r="BQ2">
-        <v>0.0425105961798564</v>
+        <v>5.329421109388364e-07</v>
       </c>
       <c r="BR2">
-        <v>-1.192969270480184e-06</v>
+        <v>-3.5435011156434e-12</v>
       </c>
       <c r="BS2">
-        <v>0.1110988883423754</v>
+        <v>4.329971215863789e-06</v>
       </c>
       <c r="BT2">
-        <v>280.8335504004829</v>
+        <v>3.473619965457054e-06</v>
       </c>
       <c r="BU2">
-        <v>0.4244989967761957</v>
+        <v>4.689936103610275e-06</v>
       </c>
       <c r="BV2">
-        <v>1.832102408542392e-08</v>
+        <v>-7.943904232665936e-09</v>
       </c>
       <c r="BW2">
-        <v>0.07873644409485463</v>
+        <v>-0.1911810796748014</v>
       </c>
       <c r="BX2">
-        <v>0.1574729065107333</v>
+        <v>-0.3823621672935071</v>
       </c>
       <c r="BY2">
-        <v>-0.1574728698686852</v>
+        <v>0.3823621514056986</v>
       </c>
       <c r="BZ2">
-        <v>-3522.713212501598</v>
+        <v>5.572654145880812</v>
       </c>
       <c r="CA2">
-        <v>-558279062.468701</v>
+        <v>1108460.637118418</v>
       </c>
       <c r="CB2">
-        <v>-7.076440304029989e-14</v>
+        <v>-0.09821790653089858</v>
       </c>
       <c r="CC2">
-        <v>-1.089015995973703e-08</v>
+        <v>-120176.5545372417</v>
       </c>
       <c r="CD2">
-        <v>-31.98665451353119</v>
+        <v>0.001326572291986015</v>
       </c>
       <c r="CE2">
-        <v>-3918891.731147497</v>
+        <v>83.58858553837233</v>
       </c>
       <c r="CF2">
-        <v>51.03558852623057</v>
+        <v>0.00385769413294626</v>
       </c>
       <c r="CG2">
-        <v>8950478.101553122</v>
+        <v>970.6686028398</v>
       </c>
     </row>
     <row r="3" spans="1:85">
@@ -1148,253 +1148,253 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>105</v>
+        <v>246</v>
       </c>
       <c r="D3">
-        <v>934</v>
+        <v>646.386</v>
       </c>
       <c r="E3">
-        <v>0.34</v>
+        <v>0.21</v>
       </c>
       <c r="F3">
-        <v>1.918581712031686e-06</v>
+        <v>1.002654632104177e-11</v>
       </c>
       <c r="G3">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
       <c r="H3">
-        <v>6.192700868401953e-07</v>
+        <v>1.293040091364891e-11</v>
       </c>
       <c r="I3">
-        <v>0.013</v>
+        <v>0.00042</v>
       </c>
       <c r="J3">
-        <v>0.002910571956654697</v>
+        <v>2.013269111875995e-11</v>
       </c>
       <c r="K3">
-        <v>0.000222</v>
+        <v>9.236016e-05</v>
       </c>
       <c r="L3">
-        <v>1.453115052870038e-06</v>
+        <v>7.650317003648775e-11</v>
       </c>
       <c r="M3">
-        <v>0.001554</v>
+        <v>0.001411058</v>
       </c>
       <c r="N3">
-        <v>933.4931</v>
+        <v>646.374006214</v>
       </c>
       <c r="O3">
-        <v>0.3400000588235243</v>
+        <v>0.2100000952380737</v>
       </c>
       <c r="P3">
-        <v>0.0003642234300644796</v>
+        <v>0.0003248894497910043</v>
       </c>
       <c r="Q3">
-        <v>15.297</v>
+        <v>0.299842</v>
       </c>
       <c r="R3">
-        <v>0.01500299970005999</v>
+        <v>0.01600281225285106</v>
       </c>
       <c r="S3">
-        <v>0.000980780525597175</v>
+        <v>0.05337081613933691</v>
       </c>
       <c r="T3">
-        <v>2.469</v>
+        <v>0.389718</v>
       </c>
       <c r="U3">
-        <v>0.01300038460969521</v>
+        <v>0.0004317406628984581</v>
       </c>
       <c r="V3">
-        <v>0.005265445366421713</v>
+        <v>0.001107828385905855</v>
       </c>
       <c r="W3">
-        <v>0.07488900000000002</v>
+        <v>0.004815007603999999</v>
       </c>
       <c r="X3">
-        <v>0.0005838527211549159</v>
+        <v>0.0008053138513369962</v>
       </c>
       <c r="Y3">
-        <v>0.007796241385983465</v>
+        <v>0.1672507953399686</v>
       </c>
       <c r="Z3">
-        <v>2.8969</v>
+        <v>2.3425746368</v>
       </c>
       <c r="AA3">
-        <v>0.001554128694799758</v>
+        <v>0.00141194358221708</v>
       </c>
       <c r="AB3">
-        <v>0.0005364799250232172</v>
+        <v>0.000602731524552755</v>
       </c>
       <c r="AC3">
-        <v>8.031712361485972</v>
+        <v>130.0430761721729</v>
       </c>
       <c r="AD3">
-        <v>19292.70616693757</v>
+        <v>0.9690721073699309</v>
       </c>
       <c r="AE3">
-        <v>9646.853083468786</v>
+        <v>0.9845360536849654</v>
       </c>
       <c r="AF3">
-        <v>4823.926541734393</v>
+        <v>0.9922680268424827</v>
       </c>
       <c r="AG3">
-        <v>55889.04049500146</v>
+        <v>2.270123739955126</v>
       </c>
       <c r="AH3">
-        <v>134035.3490093758</v>
+        <v>251555.4930038796</v>
       </c>
       <c r="AI3">
-        <v>23818.08026308443</v>
+        <v>0.3836914217699974</v>
       </c>
       <c r="AJ3">
-        <v>67017.67450468813</v>
+        <v>125777.7465019398</v>
       </c>
       <c r="AK3">
-        <v>73791.604308911</v>
+        <v>0.2975236297045037</v>
       </c>
       <c r="AL3">
-        <v>33508.83725234398</v>
+        <v>62888.87325099254</v>
       </c>
       <c r="AM3">
-        <v>111945075.2559499</v>
+        <v>0.597409232010681</v>
       </c>
       <c r="AN3">
-        <v>100526.511757032</v>
+        <v>188666.6197529514</v>
       </c>
       <c r="AO3">
-        <v>75003.20042148643</v>
+        <v>0.0004002641854471563</v>
       </c>
       <c r="AP3">
-        <v>100526.5117570332</v>
+        <v>188666.619752952</v>
       </c>
       <c r="AQ3">
-        <v>7539810108.98567</v>
+        <v>75.51649087648367</v>
       </c>
       <c r="AR3">
-        <v>-1211.596112575426</v>
+        <v>0.2971233655190565</v>
       </c>
       <c r="AS3">
-        <v>7934912580.386316</v>
+        <v>18711.0782276937</v>
       </c>
       <c r="AT3">
-        <v>28545.99419026722</v>
+        <v>0.0001523393541627236</v>
       </c>
       <c r="AU3">
-        <v>100526.5117570332</v>
+        <v>188666.619752952</v>
       </c>
       <c r="AV3">
-        <v>2869629220.584098</v>
+        <v>28.74135100522886</v>
       </c>
       <c r="AW3">
-        <v>27343.04630473424</v>
+        <v>2.269971400600963</v>
       </c>
       <c r="AX3">
-        <v>8021935968.107422</v>
+        <v>571062.0973074937</v>
       </c>
       <c r="AY3">
-        <v>293381.2084690243</v>
+        <v>251572.3753860105</v>
       </c>
       <c r="AZ3">
-        <v>8163539.904741455</v>
+        <v>677.7226613634236</v>
       </c>
       <c r="BA3">
-        <v>2395029202638.152</v>
+        <v>170496299.7721253</v>
       </c>
       <c r="BB3">
-        <v>-8162606.411641455</v>
+        <v>-31.34865514942362</v>
       </c>
       <c r="BC3">
-        <v>2395029202638.152</v>
+        <v>170496299.7721253</v>
       </c>
       <c r="BD3">
-        <v>-8744.152915154333</v>
+        <v>-0.04849925097242351</v>
       </c>
       <c r="BE3">
-        <v>8746.152915154333</v>
+        <v>2.048499250972424</v>
       </c>
       <c r="BF3">
-        <v>2565956911.702858</v>
+        <v>515345.822543596</v>
       </c>
       <c r="BG3">
-        <v>-293414.7601705231</v>
+        <v>-5438711.771189332</v>
       </c>
       <c r="BH3">
-        <v>-35102.594184579</v>
+        <v>-0.4272025407842774</v>
       </c>
       <c r="BI3">
-        <v>3395370729.417294</v>
+        <v>165570.9188135121</v>
       </c>
       <c r="BJ3">
-        <v>-96727.0598737948</v>
+        <v>-387570.070415662</v>
       </c>
       <c r="BK3">
-        <v>2.42708206e-08</v>
+        <v>2.17828040094118e-08</v>
       </c>
       <c r="BL3">
-        <v>8.840001529411632e-12</v>
+        <v>7.077003209523082e-12</v>
       </c>
       <c r="BM3">
-        <v>-0.0002122277667026779</v>
+        <v>-1.056449678535576e-09</v>
       </c>
       <c r="BN3">
-        <v>62.27075926859196</v>
+        <v>0.005745725302320623</v>
       </c>
       <c r="BO3">
-        <v>0.06428944234379325</v>
+        <v>6.305582007292016e-07</v>
       </c>
       <c r="BP3">
-        <v>5.465552761502956</v>
+        <v>5.595259288452875</v>
       </c>
       <c r="BQ3">
-        <v>0.04150204111034616</v>
+        <v>1.626356688285383e-06</v>
       </c>
       <c r="BR3">
-        <v>-9.126674487990541e-07</v>
+        <v>-1.439672562443015e-11</v>
       </c>
       <c r="BS3">
-        <v>0.08827963896484965</v>
+        <v>5.579739964015358e-06</v>
       </c>
       <c r="BT3">
-        <v>292.5896460203361</v>
+        <v>3.798366779906704e-06</v>
       </c>
       <c r="BU3">
-        <v>0.1947687832622132</v>
+        <v>1.92447926548883e-05</v>
       </c>
       <c r="BV3">
-        <v>2.591273479787102e-07</v>
+        <v>-7.326714817263614e-09</v>
       </c>
       <c r="BW3">
-        <v>99.58856587471492</v>
+        <v>-0.5018770489195951</v>
       </c>
       <c r="BX3">
-        <v>199.1771320085572</v>
+        <v>-1.003754105165905</v>
       </c>
       <c r="BY3">
-        <v>-199.1771314903025</v>
+        <v>1.003754090512475</v>
       </c>
       <c r="BZ3">
-        <v>-179245.7434803985</v>
+        <v>3.900648836809127</v>
       </c>
       <c r="CA3">
-        <v>-1174043754232.901</v>
+        <v>775835.3412343368</v>
       </c>
       <c r="CB3">
-        <v>-3.116828196049815e-13</v>
+        <v>-0.2555832366495572</v>
       </c>
       <c r="CC3">
-        <v>-2.041477048657991e-06</v>
+        <v>-100355.4982784489</v>
       </c>
       <c r="CD3">
-        <v>-1.297916516549962</v>
+        <v>0.0004596771569750991</v>
       </c>
       <c r="CE3">
-        <v>-8500236.991988815</v>
+        <v>28.94775787363404</v>
       </c>
       <c r="CF3">
-        <v>29.29110703092957</v>
+        <v>0.003511854404382448</v>
       </c>
       <c r="CG3">
-        <v>8593460.378129652</v>
+        <v>883.4855545203155</v>
       </c>
     </row>
     <row r="4" spans="1:85">
@@ -1405,91 +1405,253 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>105</v>
+        <v>246</v>
       </c>
       <c r="D4">
-        <v>438.697</v>
+        <v>113.456</v>
       </c>
       <c r="E4">
-        <v>0.083</v>
+        <v>0.036</v>
       </c>
       <c r="F4">
-        <v>4.255684396468324e-06</v>
+        <v>3.074324450117895e-11</v>
       </c>
       <c r="G4">
-        <v>0.015</v>
+        <v>0.018</v>
       </c>
       <c r="H4">
-        <v>9.713360417996839e-07</v>
+        <v>5.923157339169428e-12</v>
       </c>
       <c r="I4">
-        <v>0.013</v>
+        <v>0.00029</v>
+      </c>
+      <c r="J4">
+        <v>1.311625673222111e-11</v>
+      </c>
+      <c r="K4">
+        <v>6.450841999999999e-05</v>
+      </c>
+      <c r="L4">
+        <v>1.155691907038956e-11</v>
+      </c>
+      <c r="M4">
+        <v>0.0004381703999999999</v>
       </c>
       <c r="N4">
-        <v>437.5751813</v>
+        <v>113.423561757</v>
       </c>
       <c r="O4">
-        <v>0.08300024096350565</v>
+        <v>0.03600055555126893</v>
       </c>
       <c r="P4">
-        <v>0.0001896822409281046</v>
+        <v>0.0003173992686669191</v>
       </c>
       <c r="Q4">
-        <v>33.9309</v>
+        <v>0.919371</v>
       </c>
       <c r="R4">
-        <v>0.01500299970005999</v>
+        <v>0.018002499826413</v>
       </c>
       <c r="S4">
-        <v>0.000442163329002767</v>
+        <v>0.01958132225881934</v>
       </c>
       <c r="T4">
-        <v>3.87267</v>
+        <v>0.178522</v>
       </c>
       <c r="U4">
-        <v>0.01300038460969521</v>
+        <v>0.0003067572330035594</v>
       </c>
       <c r="V4">
-        <v>0.003356956469230584</v>
+        <v>0.001718316134726025</v>
+      </c>
+      <c r="W4">
+        <v>0.0031369316466</v>
+      </c>
+      <c r="X4">
+        <v>0.000802596621130999</v>
+      </c>
+      <c r="Y4">
+        <v>0.255854035583116</v>
+      </c>
+      <c r="Z4">
+        <v>0.3538800481199999</v>
+      </c>
+      <c r="AA4">
+        <v>0.0004410139447184861</v>
+      </c>
+      <c r="AB4">
+        <v>0.001246224383265991</v>
       </c>
       <c r="AC4">
-        <v>8.031712361485972</v>
+        <v>130.0430761721729</v>
       </c>
       <c r="AD4">
-        <v>19292.70616693757</v>
+        <v>0.9690721073699309</v>
       </c>
       <c r="AE4">
-        <v>9646.853083468786</v>
+        <v>0.9845360536849654</v>
       </c>
       <c r="AF4">
-        <v>4823.926541734393</v>
+        <v>0.9922680268424827</v>
+      </c>
+      <c r="AG4">
+        <v>0.3429352839878209</v>
+      </c>
+      <c r="AH4">
+        <v>251555.4930038796</v>
       </c>
       <c r="AI4">
-        <v>37359.07853075707</v>
+        <v>0.1757613453759474</v>
       </c>
       <c r="AJ4">
-        <v>67017.67450468801</v>
+        <v>125777.7465019398</v>
       </c>
       <c r="AK4">
-        <v>163680.1690949355</v>
+        <v>0.9122624481062003</v>
       </c>
       <c r="AL4">
-        <v>33508.83725234396</v>
+        <v>62888.87325097294</v>
+      </c>
+      <c r="AM4">
+        <v>0.3892064312231785</v>
+      </c>
+      <c r="AN4">
+        <v>188666.6197530073</v>
+      </c>
+      <c r="AO4">
+        <v>0.0002607683089195296</v>
+      </c>
+      <c r="AP4">
+        <v>188666.6197530078</v>
+      </c>
+      <c r="AQ4">
+        <v>49.19827538255577</v>
+      </c>
+      <c r="AR4">
+        <v>0.9120016797972808</v>
+      </c>
+      <c r="AS4">
+        <v>57371.17856540509</v>
+      </c>
+      <c r="AT4">
+        <v>9.924763996191053e-05</v>
+      </c>
+      <c r="AU4">
+        <v>188666.6197530078</v>
+      </c>
+      <c r="AV4">
+        <v>18.7247167500772</v>
+      </c>
+      <c r="AW4">
+        <v>0.342836036347859</v>
+      </c>
+      <c r="AX4">
+        <v>86267.25646412598</v>
+      </c>
+      <c r="AY4">
+        <v>251628.3217572694</v>
+      </c>
+      <c r="AZ4">
+        <v>102.3571270120168</v>
+      </c>
+      <c r="BA4">
+        <v>25755952.08992945</v>
+      </c>
+      <c r="BB4">
+        <v>11.06643474498323</v>
+      </c>
+      <c r="BC4">
+        <v>25755952.08992945</v>
+      </c>
+      <c r="BD4">
+        <v>0.0975673358652948</v>
+      </c>
+      <c r="BE4">
+        <v>1.902432664134705</v>
+      </c>
+      <c r="BF4">
+        <v>478705.9385324269</v>
+      </c>
+      <c r="BG4">
+        <v>2327393.843044659</v>
+      </c>
+      <c r="BH4">
+        <v>-0.0729272685500561</v>
+      </c>
+      <c r="BI4">
+        <v>126826.9300381862</v>
+      </c>
+      <c r="BJ4">
+        <v>-1739087.896198035</v>
       </c>
       <c r="BK4">
-        <v>1.13769547138e-08</v>
+        <v>3.8223740312109e-09</v>
       </c>
       <c r="BL4">
-        <v>2.158006265051147e-12</v>
+        <v>1.213218722077763e-12</v>
+      </c>
+      <c r="BM4">
+        <v>3.729388509059347e-10</v>
+      </c>
+      <c r="BN4">
+        <v>0.0008679755854306226</v>
       </c>
       <c r="BO4">
-        <v>0.1426030358385967</v>
+        <v>1.933408006758314e-06</v>
       </c>
       <c r="BP4">
-        <v>12.12336564001312</v>
+        <v>17.15609930324707</v>
       </c>
       <c r="BQ4">
-        <v>0.06509668268400325</v>
+        <v>7.450013822971565e-07</v>
+      </c>
+      <c r="BR4">
+        <v>-2.45764895013689e-12</v>
+      </c>
+      <c r="BS4">
+        <v>4.274067542286875e-06</v>
+      </c>
+      <c r="BT4">
+        <v>2.474599821480782e-06</v>
+      </c>
+      <c r="BU4">
+        <v>2.907206474357784e-06</v>
+      </c>
+      <c r="BV4">
+        <v>8.426346283843306e-10</v>
+      </c>
+      <c r="BW4">
+        <v>0.02467387230319173</v>
+      </c>
+      <c r="BX4">
+        <v>0.04934774544901809</v>
+      </c>
+      <c r="BY4">
+        <v>-0.04934774376374883</v>
+      </c>
+      <c r="BZ4">
+        <v>0.8279156643009701</v>
+      </c>
+      <c r="CA4">
+        <v>164654.0238335137</v>
+      </c>
+      <c r="CB4">
+        <v>-0.01422951676774358</v>
+      </c>
+      <c r="CC4">
+        <v>-24762.56464144402</v>
+      </c>
+      <c r="CD4">
+        <v>0.008040672199583753</v>
+      </c>
+      <c r="CE4">
+        <v>505.8135864955272</v>
+      </c>
+      <c r="CF4">
+        <v>0.003022617444181086</v>
+      </c>
+      <c r="CG4">
+        <v>760.5761547935339</v>
       </c>
     </row>
     <row r="5" spans="1:85">
@@ -1500,253 +1662,253 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>105</v>
+        <v>246</v>
       </c>
       <c r="D5">
-        <v>144</v>
+        <v>140.526</v>
       </c>
       <c r="E5">
-        <v>0.024</v>
+        <v>0.047</v>
       </c>
       <c r="F5">
-        <v>1.680279740870007e-06</v>
+        <v>5.674571377731692e-11</v>
       </c>
       <c r="G5">
-        <v>0.013</v>
+        <v>0.017</v>
       </c>
       <c r="H5">
-        <v>3.784846338768144e-07</v>
+        <v>9.536003950019399e-12</v>
       </c>
       <c r="I5">
-        <v>0.011</v>
+        <v>0.0004</v>
       </c>
       <c r="J5">
-        <v>0.001246444113579735</v>
+        <v>1.448291083943797e-11</v>
       </c>
       <c r="K5">
-        <v>0.0001526</v>
+        <v>6.661380000000001e-05</v>
       </c>
       <c r="L5">
-        <v>1.02142917676111e-07</v>
+        <v>1.362140387009064e-11</v>
       </c>
       <c r="M5">
-        <v>0.0003379</v>
+        <v>0.0005207988</v>
       </c>
       <c r="N5">
-        <v>143.5558</v>
+        <v>140.46790099</v>
       </c>
       <c r="O5">
-        <v>0.02400083331886624</v>
+        <v>0.04700042552998856</v>
       </c>
       <c r="P5">
-        <v>0.0001671881827057231</v>
+        <v>0.0003345990450397244</v>
       </c>
       <c r="Q5">
-        <v>13.397</v>
+        <v>1.69697</v>
       </c>
       <c r="R5">
-        <v>0.0130034610777285</v>
+        <v>0.01700264685276972</v>
       </c>
       <c r="S5">
-        <v>0.0009706248471843322</v>
+        <v>0.01001941510620089</v>
       </c>
       <c r="T5">
-        <v>1.509</v>
+        <v>0.287412</v>
       </c>
       <c r="U5">
-        <v>0.0110004545360635</v>
+        <v>0.000412310562561766</v>
       </c>
       <c r="V5">
-        <v>0.007289896975522529</v>
+        <v>0.001434562796827432</v>
       </c>
       <c r="W5">
-        <v>0.032071</v>
+        <v>0.0034637856116</v>
       </c>
       <c r="X5">
-        <v>0.0005611477167377588</v>
+        <v>0.0008027685833105579</v>
       </c>
       <c r="Y5">
-        <v>0.01749704458039222</v>
+        <v>0.2317604705736222</v>
       </c>
       <c r="Z5">
-        <v>0.20363</v>
+        <v>0.4170958564</v>
       </c>
       <c r="AA5">
-        <v>0.0003384913735976148</v>
+        <v>0.0005231934537830534</v>
       </c>
       <c r="AB5">
-        <v>0.001662286370365932</v>
+        <v>0.00125437221625454</v>
       </c>
       <c r="AC5">
-        <v>8.031712361485972</v>
+        <v>130.0430761721729</v>
       </c>
       <c r="AD5">
-        <v>19292.70616693757</v>
+        <v>0.9690721073699309</v>
       </c>
       <c r="AE5">
-        <v>9646.853083468786</v>
+        <v>0.9845360536849654</v>
       </c>
       <c r="AF5">
-        <v>4823.926541734393</v>
+        <v>0.9922680268424827</v>
       </c>
       <c r="AG5">
-        <v>3928.573756773499</v>
+        <v>0.4041959605368141</v>
       </c>
       <c r="AH5">
-        <v>134035.3490093758</v>
+        <v>251555.4930038796</v>
       </c>
       <c r="AI5">
-        <v>14557.1013029544</v>
+        <v>0.2829674762617033</v>
       </c>
       <c r="AJ5">
-        <v>67017.67450468832</v>
+        <v>125777.7465019398</v>
       </c>
       <c r="AK5">
-        <v>64626.14387961567</v>
+        <v>1.683849073510888</v>
       </c>
       <c r="AL5">
-        <v>33508.83725234398</v>
+        <v>62888.87325097069</v>
       </c>
       <c r="AM5">
-        <v>47940158.21460519</v>
+        <v>0.4297599655619576</v>
       </c>
       <c r="AN5">
-        <v>100526.5117570327</v>
+        <v>188666.6197529897</v>
       </c>
       <c r="AO5">
-        <v>32119.90600378548</v>
+        <v>0.0002879391769265116</v>
       </c>
       <c r="AP5">
-        <v>100526.5117570338</v>
+        <v>188666.6197529903</v>
       </c>
       <c r="AQ5">
-        <v>3228902108.524363</v>
+        <v>54.32451120518316</v>
       </c>
       <c r="AR5">
-        <v>32506.23787583019</v>
+        <v>1.683561134333961</v>
       </c>
       <c r="AS5">
-        <v>3887853182.025523</v>
+        <v>105895.3848920746</v>
       </c>
       <c r="AT5">
-        <v>12224.74034472433</v>
+        <v>0.0001095887912182992</v>
       </c>
       <c r="AU5">
-        <v>100526.5117570338</v>
+        <v>188666.6197529903</v>
       </c>
       <c r="AV5">
-        <v>1228910503.990616</v>
+        <v>20.6757468019727</v>
       </c>
       <c r="AW5">
-        <v>-8296.166587950825</v>
+        <v>0.4040863717455958</v>
       </c>
       <c r="AX5">
-        <v>1336972186.322913</v>
+        <v>101677.7162251791</v>
       </c>
       <c r="AY5">
-        <v>-161155.4170410106</v>
+        <v>251623.7204089458</v>
       </c>
       <c r="AZ5">
-        <v>-2476903.496498598</v>
+        <v>120.6440271483651</v>
       </c>
       <c r="BA5">
-        <v>399166415948.569</v>
+        <v>30356898.95618948</v>
       </c>
       <c r="BB5">
-        <v>2477047.052298598</v>
+        <v>19.82387384163492</v>
       </c>
       <c r="BC5">
-        <v>399166415948.569</v>
+        <v>30356898.95618948</v>
       </c>
       <c r="BD5">
-        <v>17254.94234505745</v>
+        <v>0.1411274298392641</v>
       </c>
       <c r="BE5">
-        <v>-17252.94234505745</v>
+        <v>1.858872570160736</v>
       </c>
       <c r="BF5">
-        <v>2780405118.802245</v>
+        <v>467736.4318699834</v>
       </c>
       <c r="BG5">
-        <v>161146.0773739275</v>
+        <v>1531330.314079817</v>
       </c>
       <c r="BH5">
-        <v>-11579.03535859501</v>
+        <v>-0.09186867233969224</v>
       </c>
       <c r="BI5">
-        <v>1326182217.305674</v>
+        <v>127236.5281907174</v>
       </c>
       <c r="BJ5">
-        <v>-114533.0484133345</v>
+        <v>-1384982.768883929</v>
       </c>
       <c r="BK5">
-        <v>3.732450800000001e-09</v>
+        <v>4.733768263363e-09</v>
       </c>
       <c r="BL5">
-        <v>6.240216662905224e-13</v>
+        <v>1.583914340360614e-12</v>
       </c>
       <c r="BM5">
-        <v>6.440322335976356e-05</v>
+        <v>6.680645484630967e-10</v>
       </c>
       <c r="BN5">
-        <v>10.3783268146628</v>
+        <v>0.001023027494823585</v>
       </c>
       <c r="BO5">
-        <v>0.05630422037522378</v>
+        <v>3.568674001277545e-06</v>
       </c>
       <c r="BP5">
-        <v>4.786690877025241</v>
+        <v>31.66663494348983</v>
       </c>
       <c r="BQ5">
-        <v>0.02536515999818247</v>
+        <v>1.199417087467036e-06</v>
       </c>
       <c r="BR5">
-        <v>-3.010549193234701e-07</v>
+        <v>-3.095974257847628e-12</v>
       </c>
       <c r="BS5">
-        <v>0.03448073764994753</v>
+        <v>4.287871000027174e-06</v>
       </c>
       <c r="BT5">
-        <v>125.3006788382575</v>
+        <v>2.732441832260696e-06</v>
       </c>
       <c r="BU5">
-        <v>0.01369076161955348</v>
+        <v>3.426538965945603e-06</v>
       </c>
       <c r="BV5">
-        <v>2.93095991491651e-09</v>
+        <v>8.176863627294799e-10</v>
       </c>
       <c r="BW5">
-        <v>0.01129803094591165</v>
+        <v>0.01575192996088047</v>
       </c>
       <c r="BX5">
-        <v>0.02259606482278322</v>
+        <v>0.0315038607394473</v>
       </c>
       <c r="BY5">
-        <v>-0.02259605896086338</v>
+        <v>-0.03150385910407458</v>
       </c>
       <c r="BZ5">
-        <v>2861.109528934031</v>
+        <v>0.4952207057928038</v>
       </c>
       <c r="CA5">
-        <v>447016001.6775844</v>
+        <v>98487.25712551545</v>
       </c>
       <c r="CB5">
-        <v>-9.004245376546968e-14</v>
+        <v>-0.009711454508431323</v>
       </c>
       <c r="CC5">
-        <v>-1.491086926959706e-08</v>
+        <v>-13464.06095964823</v>
       </c>
       <c r="CD5">
-        <v>226.4362559773286</v>
+        <v>0.01198537973777949</v>
       </c>
       <c r="CE5">
-        <v>27082522.48969058</v>
+        <v>753.8760396199934</v>
       </c>
       <c r="CF5">
-        <v>-57.79053572165544</v>
+        <v>0.002876716807880278</v>
       </c>
       <c r="CG5">
-        <v>-9313257.885246806</v>
+        <v>723.8501857617821</v>
       </c>
     </row>
     <row r="6" spans="1:85">
@@ -1757,728 +1919,253 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>105</v>
+        <v>246</v>
       </c>
       <c r="D6">
-        <v>175</v>
+        <v>341.902</v>
       </c>
       <c r="E6">
-        <v>0.031</v>
+        <v>0.11</v>
       </c>
       <c r="F6">
-        <v>2.156883683193366e-06</v>
+        <v>7.525978997780914e-11</v>
       </c>
       <c r="G6">
-        <v>0.014</v>
+        <v>0.017</v>
       </c>
       <c r="H6">
-        <v>4.913528149533992e-07</v>
+        <v>1.558281891907805e-11</v>
       </c>
       <c r="I6">
-        <v>0.012</v>
+        <v>0.00043</v>
       </c>
       <c r="J6">
-        <v>0.001446949404401906</v>
+        <v>1.434228908477918e-11</v>
       </c>
       <c r="K6">
-        <v>0.000165</v>
+        <v>7.913705e-05</v>
       </c>
       <c r="L6">
-        <v>1.152198997701846e-07</v>
+        <v>3.481026330992743e-11</v>
       </c>
       <c r="M6">
-        <v>0.000374</v>
+        <v>0.0008149934999999998</v>
       </c>
       <c r="N6">
-        <v>174.4304</v>
+        <v>341.82563021</v>
       </c>
       <c r="O6">
-        <v>0.03100064515457703</v>
+        <v>0.1100001818180315</v>
       </c>
       <c r="P6">
-        <v>0.0001777250132693443</v>
+        <v>0.0003218020303230426</v>
       </c>
       <c r="Q6">
-        <v>17.197</v>
+        <v>2.25063</v>
       </c>
       <c r="R6">
-        <v>0.0140032139168121</v>
+        <v>0.01700264685276972</v>
       </c>
       <c r="S6">
-        <v>0.0008142823699954701</v>
+        <v>0.007554616641904588</v>
       </c>
       <c r="T6">
-        <v>1.959</v>
+        <v>0.469661</v>
       </c>
       <c r="U6">
-        <v>0.01200041665943312</v>
+        <v>0.0004414748010928823</v>
       </c>
       <c r="V6">
-        <v>0.006125786962446718</v>
+        <v>0.0009399860773896115</v>
       </c>
       <c r="W6">
-        <v>0.03723000000000001</v>
+        <v>0.0034301540015</v>
       </c>
       <c r="X6">
-        <v>0.0005646459067415613</v>
+        <v>0.0008039046415357374</v>
       </c>
       <c r="Y6">
-        <v>0.01516642242120766</v>
+        <v>0.2343640084918028</v>
       </c>
       <c r="Z6">
-        <v>0.2297</v>
+        <v>1.06591190785</v>
       </c>
       <c r="AA6">
-        <v>0.0003745343775943671</v>
+        <v>0.0008165258140697388</v>
       </c>
       <c r="AB6">
-        <v>0.001630537124921059</v>
+        <v>0.0007660349866216563</v>
       </c>
       <c r="AC6">
-        <v>8.031712361485972</v>
+        <v>130.0430761721729</v>
       </c>
       <c r="AD6">
-        <v>19292.70616693757</v>
+        <v>0.9690721073699309</v>
       </c>
       <c r="AE6">
-        <v>9646.853083468786</v>
+        <v>0.9845360536849654</v>
       </c>
       <c r="AF6">
-        <v>4823.926541734393</v>
+        <v>0.9922680268424827</v>
       </c>
       <c r="AG6">
-        <v>4431.534606545561</v>
+        <v>1.032945498810903</v>
       </c>
       <c r="AH6">
-        <v>134035.3490093758</v>
+        <v>251555.4930038796</v>
       </c>
       <c r="AI6">
-        <v>18898.18519051535</v>
+        <v>0.4623981875097345</v>
       </c>
       <c r="AJ6">
-        <v>67017.6745046882</v>
+        <v>125777.7465019398</v>
       </c>
       <c r="AK6">
-        <v>82957.06473820636</v>
+        <v>2.233228189252497</v>
       </c>
       <c r="AL6">
-        <v>33508.83725234397</v>
+        <v>62888.87325097034</v>
       </c>
       <c r="AM6">
-        <v>55651900.16930409</v>
+        <v>0.4255872131981954</v>
       </c>
       <c r="AN6">
-        <v>100526.5117570325</v>
+        <v>188666.6197529915</v>
       </c>
       <c r="AO6">
-        <v>37286.77311343374</v>
+        <v>0.0002851434328427909</v>
       </c>
       <c r="AP6">
-        <v>100526.5117570336</v>
+        <v>188666.6197529921</v>
       </c>
       <c r="AQ6">
-        <v>3748309235.769443</v>
+        <v>53.79704761921368</v>
       </c>
       <c r="AR6">
-        <v>45670.29162477262</v>
+        <v>2.232943045819654</v>
       </c>
       <c r="AS6">
-        <v>4666592027.678216</v>
+        <v>140445.21483778</v>
       </c>
       <c r="AT6">
-        <v>14191.23454317254</v>
+        <v>0.0001085247393655398</v>
       </c>
       <c r="AU6">
-        <v>100526.5117570336</v>
+        <v>188666.6197529921</v>
       </c>
       <c r="AV6">
-        <v>1426595306.151057</v>
+        <v>20.47499573567088</v>
       </c>
       <c r="AW6">
-        <v>-9759.699936626981</v>
+        <v>1.032836974071538</v>
       </c>
       <c r="AX6">
-        <v>1545311983.243799</v>
+        <v>259843.1150062045</v>
       </c>
       <c r="AY6">
-        <v>-158336.0137379254</v>
+        <v>251581.9258308301</v>
       </c>
       <c r="AZ6">
-        <v>-2913856.013079351</v>
+        <v>308.3638069787983</v>
       </c>
       <c r="BA6">
-        <v>461368345717.2686</v>
+        <v>77578760.41625243</v>
       </c>
       <c r="BB6">
-        <v>2914030.443479351</v>
+        <v>33.46182323120172</v>
       </c>
       <c r="BC6">
-        <v>461368345717.2686</v>
+        <v>77578760.41625243</v>
       </c>
       <c r="BD6">
-        <v>16705.97810633554</v>
+        <v>0.09789149868792608</v>
       </c>
       <c r="BE6">
-        <v>-16703.97810633554</v>
+        <v>1.902108501312074</v>
       </c>
       <c r="BF6">
-        <v>2644841306.922749</v>
+        <v>478536.1198992855</v>
       </c>
       <c r="BG6">
-        <v>158326.5359322722</v>
+        <v>2318425.982954615</v>
       </c>
       <c r="BH6">
-        <v>-13483.28947193061</v>
+        <v>-0.2145290406566399</v>
       </c>
       <c r="BI6">
-        <v>1539336976.501683</v>
+        <v>134993.0635528537</v>
       </c>
       <c r="BJ6">
-        <v>-114166.2781701943</v>
+        <v>-629253.0985066686</v>
       </c>
       <c r="BK6">
-        <v>4.5351904e-09</v>
+        <v>1.1519523738077e-08</v>
       </c>
       <c r="BL6">
-        <v>8.060167740190027e-13</v>
+        <v>3.707006127267663e-12</v>
       </c>
       <c r="BM6">
-        <v>7.576479153046314e-05</v>
+        <v>1.127663442891498e-09</v>
       </c>
       <c r="BN6">
-        <v>11.99557698864898</v>
+        <v>0.002614404226027707</v>
       </c>
       <c r="BO6">
-        <v>0.07227466431236272</v>
+        <v>4.733003392809087e-06</v>
       </c>
       <c r="BP6">
-        <v>6.144414645980674</v>
+        <v>41.99831381984743</v>
       </c>
       <c r="BQ6">
-        <v>0.0329293230195092</v>
+        <v>1.95997184778943e-06</v>
       </c>
       <c r="BR6">
-        <v>-3.505655262701959e-07</v>
+        <v>-7.229628670128764e-12</v>
       </c>
       <c r="BS6">
-        <v>0.04002276138904376</v>
+        <v>4.54926624173117e-06</v>
       </c>
       <c r="BT6">
-        <v>145.4567763134395</v>
+        <v>2.705911201145515e-06</v>
       </c>
       <c r="BU6">
-        <v>0.01544353947852199</v>
+        <v>8.756712948523654e-06</v>
       </c>
       <c r="BV6">
-        <v>2.454158651063498e-09</v>
+        <v>1.040636687390844e-09</v>
       </c>
       <c r="BW6">
-        <v>0.007940583008581036</v>
+        <v>0.03034950866805062</v>
       </c>
       <c r="BX6">
-        <v>0.01588116847132072</v>
+        <v>0.06069901837673792</v>
       </c>
       <c r="BY6">
-        <v>-0.01588116356300342</v>
+        <v>-0.06069901629546454</v>
       </c>
       <c r="BZ6">
-        <v>2364.0025602527</v>
+        <v>0.3697538077158743</v>
       </c>
       <c r="CA6">
-        <v>338855992.222844</v>
+        <v>73534.64804973207</v>
       </c>
       <c r="CB6">
-        <v>-1.34590973303406e-13</v>
+        <v>-0.01709908974848805</v>
       </c>
       <c r="CC6">
-        <v>-2.062129559797965e-08</v>
+        <v>-10813.27134291314</v>
       </c>
       <c r="CD6">
-        <v>261.8252989431465</v>
+        <v>0.006532403800288028</v>
       </c>
       <c r="CE6">
-        <v>26753318.38761028</v>
+        <v>410.8680052794686</v>
       </c>
       <c r="CF6">
-        <v>-55.95182913429644</v>
+        <v>0.00302153168981804</v>
       </c>
       <c r="CG6">
-        <v>-8859189.586470013</v>
-      </c>
-    </row>
-    <row r="7" spans="1:85">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>105</v>
-      </c>
-      <c r="D7">
-        <v>233.281</v>
-      </c>
-      <c r="E7">
-        <v>0.032</v>
-      </c>
-      <c r="F7">
-        <v>3.267107482417611e-06</v>
-      </c>
-      <c r="G7">
-        <v>0.016</v>
-      </c>
-      <c r="H7">
-        <v>7.261763197741347e-07</v>
-      </c>
-      <c r="I7">
-        <v>0.014</v>
-      </c>
-      <c r="N7">
-        <v>232.4192873</v>
-      </c>
-      <c r="O7">
-        <v>0.0320006249938966</v>
-      </c>
-      <c r="P7">
-        <v>0.0001376848942514445</v>
-      </c>
-      <c r="Q7">
-        <v>26.0489</v>
-      </c>
-      <c r="R7">
-        <v>0.01600281225285106</v>
-      </c>
-      <c r="S7">
-        <v>0.0006143373521665428</v>
-      </c>
-      <c r="T7">
-        <v>2.89523</v>
-      </c>
-      <c r="U7">
-        <v>0.01400035713830187</v>
-      </c>
-      <c r="V7">
-        <v>0.004835663190248051</v>
-      </c>
-      <c r="AC7">
-        <v>8.031712361485972</v>
-      </c>
-      <c r="AD7">
-        <v>19292.70616693757</v>
-      </c>
-      <c r="AE7">
-        <v>9646.853083468786</v>
-      </c>
-      <c r="AF7">
-        <v>4823.926541734393</v>
-      </c>
-      <c r="AI7">
-        <v>27929.85845285133</v>
-      </c>
-      <c r="AJ7">
-        <v>67017.6745046881</v>
-      </c>
-      <c r="AK7">
-        <v>125657.980092985</v>
-      </c>
-      <c r="AL7">
-        <v>33508.83725234397</v>
-      </c>
-      <c r="BK7">
-        <v>6.0429014698e-09</v>
-      </c>
-      <c r="BL7">
-        <v>8.320162498413117e-13</v>
-      </c>
-      <c r="BO7">
-        <v>0.1094769729142469</v>
-      </c>
-      <c r="BP7">
-        <v>9.307160706616616</v>
-      </c>
-      <c r="BQ7">
-        <v>0.04866664823163526</v>
-      </c>
-    </row>
-    <row r="8" spans="1:85">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>105</v>
-      </c>
-      <c r="D8">
-        <v>350.337</v>
-      </c>
-      <c r="E8">
-        <v>0.05</v>
-      </c>
-      <c r="F8">
-        <v>5.633596562561185e-06</v>
-      </c>
-      <c r="G8">
-        <v>0.014</v>
-      </c>
-      <c r="H8">
-        <v>1.223290428326043e-06</v>
-      </c>
-      <c r="I8">
-        <v>0.013</v>
-      </c>
-      <c r="N8">
-        <v>348.8526367</v>
-      </c>
-      <c r="O8">
-        <v>0.05000039999840002</v>
-      </c>
-      <c r="P8">
-        <v>0.0001433281412787442</v>
-      </c>
-      <c r="Q8">
-        <v>44.9171</v>
-      </c>
-      <c r="R8">
-        <v>0.0140032139168121</v>
-      </c>
-      <c r="S8">
-        <v>0.0003117568568944144</v>
-      </c>
-      <c r="T8">
-        <v>4.877199999999999</v>
-      </c>
-      <c r="U8">
-        <v>0.01300038460969521</v>
-      </c>
-      <c r="V8">
-        <v>0.002665542649408515</v>
-      </c>
-      <c r="AC8">
-        <v>8.031712361485972</v>
-      </c>
-      <c r="AD8">
-        <v>19292.70616693757</v>
-      </c>
-      <c r="AE8">
-        <v>9646.853083468786</v>
-      </c>
-      <c r="AF8">
-        <v>4823.926541734393</v>
-      </c>
-      <c r="AI8">
-        <v>47049.63185869396</v>
-      </c>
-      <c r="AJ8">
-        <v>67017.67450468797</v>
-      </c>
-      <c r="AK8">
-        <v>216676.7908677379</v>
-      </c>
-      <c r="AL8">
-        <v>33508.83725234396</v>
-      </c>
-      <c r="BK8">
-        <v>9.070168554200001e-09</v>
-      </c>
-      <c r="BL8">
-        <v>1.300010399958401e-12</v>
-      </c>
-      <c r="BO8">
-        <v>0.1887752703602271</v>
-      </c>
-      <c r="BP8">
-        <v>16.04868797435474</v>
-      </c>
-      <c r="BQ8">
-        <v>0.08198207975025507</v>
-      </c>
-    </row>
-    <row r="9" spans="1:85">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>105</v>
-      </c>
-      <c r="D9">
-        <v>576.2479999999999</v>
-      </c>
-      <c r="E9">
-        <v>0.14</v>
-      </c>
-      <c r="F9">
-        <v>6.926460009367344e-06</v>
-      </c>
-      <c r="G9">
-        <v>0.019</v>
-      </c>
-      <c r="H9">
-        <v>1.515262855498556e-06</v>
-      </c>
-      <c r="I9">
-        <v>0.012</v>
-      </c>
-      <c r="N9">
-        <v>574.4234693999999</v>
-      </c>
-      <c r="O9">
-        <v>0.14000014285707</v>
-      </c>
-      <c r="P9">
-        <v>0.000243722880966726</v>
-      </c>
-      <c r="Q9">
-        <v>55.22519999999999</v>
-      </c>
-      <c r="R9">
-        <v>0.01900236827345476</v>
-      </c>
-      <c r="S9">
-        <v>0.000344088718075349</v>
-      </c>
-      <c r="T9">
-        <v>6.04128</v>
-      </c>
-      <c r="U9">
-        <v>0.01200041665943312</v>
-      </c>
-      <c r="V9">
-        <v>0.001986402990663091</v>
-      </c>
-      <c r="AC9">
-        <v>8.031712361485972</v>
-      </c>
-      <c r="AD9">
-        <v>19292.70616693757</v>
-      </c>
-      <c r="AE9">
-        <v>9646.853083468786</v>
-      </c>
-      <c r="AF9">
-        <v>4823.926541734393</v>
-      </c>
-      <c r="AI9">
-        <v>58279.34059609831</v>
-      </c>
-      <c r="AJ9">
-        <v>67017.67450468795</v>
-      </c>
-      <c r="AK9">
-        <v>266402.3080525902</v>
-      </c>
-      <c r="AL9">
-        <v>33508.83725234396</v>
-      </c>
-      <c r="BK9">
-        <v>1.49350102044e-08</v>
-      </c>
-      <c r="BL9">
-        <v>3.64000371428382e-12</v>
-      </c>
-      <c r="BO9">
-        <v>0.2320976211887592</v>
-      </c>
-      <c r="BP9">
-        <v>19.73172807508355</v>
-      </c>
-      <c r="BQ9">
-        <v>0.1015493928388462</v>
-      </c>
-    </row>
-    <row r="10" spans="1:85">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>105</v>
-      </c>
-      <c r="D10">
-        <v>276.099</v>
-      </c>
-      <c r="E10">
-        <v>0.038</v>
-      </c>
-      <c r="F10">
-        <v>4.021910162758717e-06</v>
-      </c>
-      <c r="G10">
-        <v>0.016</v>
-      </c>
-      <c r="H10">
-        <v>8.723305815411052e-07</v>
-      </c>
-      <c r="I10">
-        <v>0.014</v>
-      </c>
-      <c r="N10">
-        <v>275.03869</v>
-      </c>
-      <c r="O10">
-        <v>0.03800052631214468</v>
-      </c>
-      <c r="P10">
-        <v>0.0001381642935840942</v>
-      </c>
-      <c r="Q10">
-        <v>32.067</v>
-      </c>
-      <c r="R10">
-        <v>0.01600281225285106</v>
-      </c>
-      <c r="S10">
-        <v>0.0004990430115960662</v>
-      </c>
-      <c r="T10">
-        <v>3.47794</v>
-      </c>
-      <c r="U10">
-        <v>0.01400035713830187</v>
-      </c>
-      <c r="V10">
-        <v>0.0040254740272408</v>
-      </c>
-      <c r="AC10">
-        <v>8.031712361485972</v>
-      </c>
-      <c r="AD10">
-        <v>19292.70616693757</v>
-      </c>
-      <c r="AE10">
-        <v>9646.853083468786</v>
-      </c>
-      <c r="AF10">
-        <v>4823.926541734393</v>
-      </c>
-      <c r="AI10">
-        <v>33551.17621311943</v>
-      </c>
-      <c r="AJ10">
-        <v>67017.67450468804</v>
-      </c>
-      <c r="AK10">
-        <v>154688.8524137968</v>
-      </c>
-      <c r="AL10">
-        <v>33508.83725234396</v>
-      </c>
-      <c r="BK10">
-        <v>7.151005939999999e-09</v>
-      </c>
-      <c r="BL10">
-        <v>9.880136841157616e-13</v>
-      </c>
-      <c r="BO10">
-        <v>0.1347695330874301</v>
-      </c>
-      <c r="BP10">
-        <v>11.45740213134048</v>
-      </c>
-      <c r="BQ10">
-        <v>0.05846156697420701</v>
-      </c>
-    </row>
-    <row r="11" spans="1:85">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>105</v>
-      </c>
-      <c r="D11">
-        <v>343.11</v>
-      </c>
-      <c r="E11">
-        <v>0.04</v>
-      </c>
-      <c r="F11">
-        <v>4.909409414409853e-06</v>
-      </c>
-      <c r="G11">
-        <v>0.016</v>
-      </c>
-      <c r="H11">
-        <v>1.065177155728558e-06</v>
-      </c>
-      <c r="I11">
-        <v>0.014</v>
-      </c>
-      <c r="N11">
-        <v>341.8161787</v>
-      </c>
-      <c r="O11">
-        <v>0.04000049999687504</v>
-      </c>
-      <c r="P11">
-        <v>0.0001170234251316175</v>
-      </c>
-      <c r="Q11">
-        <v>39.1431</v>
-      </c>
-      <c r="R11">
-        <v>0.01600281225285106</v>
-      </c>
-      <c r="S11">
-        <v>0.0004088284334365713</v>
-      </c>
-      <c r="T11">
-        <v>4.24681</v>
-      </c>
-      <c r="U11">
-        <v>0.01400035713830187</v>
-      </c>
-      <c r="V11">
-        <v>0.003296676125916127</v>
-      </c>
-      <c r="AC11">
-        <v>8.031712361485972</v>
-      </c>
-      <c r="AD11">
-        <v>19292.70616693757</v>
-      </c>
-      <c r="AE11">
-        <v>9646.853083468786</v>
-      </c>
-      <c r="AF11">
-        <v>4823.926541734393</v>
-      </c>
-      <c r="AI11">
-        <v>40968.35214340607</v>
-      </c>
-      <c r="AJ11">
-        <v>67017.674504688</v>
-      </c>
-      <c r="AK11">
-        <v>188823.4390157635</v>
-      </c>
-      <c r="AL11">
-        <v>33508.83725234396</v>
-      </c>
-      <c r="BK11">
-        <v>8.887220646199999e-09</v>
-      </c>
-      <c r="BL11">
-        <v>1.040012999918751e-12</v>
-      </c>
-      <c r="BO11">
-        <v>0.164508601072585</v>
-      </c>
-      <c r="BP11">
-        <v>13.98566243699983</v>
-      </c>
-      <c r="BQ11">
-        <v>0.07138569591244585</v>
+        <v>760.1627614833047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>